<commit_message>
feat: Correcciones en script de carga y archivos de prueba para actividades de ETL
</commit_message>
<xml_diff>
--- a/ejercicio_ventas/datos.xlsx
+++ b/ejercicio_ventas/datos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ventas" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Clientes" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Ventas" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Clientes" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -450,6 +450,11 @@
           <t>precio</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>id_pedido</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -463,6 +468,9 @@
       <c r="C2" t="n">
         <v>1200</v>
       </c>
+      <c r="D2" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -476,6 +484,9 @@
       <c r="C3" t="n">
         <v>25</v>
       </c>
+      <c r="D3" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -483,11 +494,14 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Teclado</t>
+          <t>Mouse</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="5">
@@ -496,11 +510,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Monitor</t>
+          <t>Teclado</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>300</v>
+        <v>80</v>
+      </c>
+      <c r="D5" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="6">
@@ -509,11 +526,30 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Monitor</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>300</v>
+      </c>
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
           <t>Audífonos</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="C7" t="n">
         <v>150</v>
+      </c>
+      <c r="D7" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>